<commit_message>
updated install script, fixed various formatting, updated values
</commit_message>
<xml_diff>
--- a/source/pages.xlsx
+++ b/source/pages.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/admin/website/github/website/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679369C7-C4B2-634D-829D-D0B47F9D7DFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E91007-B740-A14B-8FF4-70236A08F548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42420" yWindow="-1180" windowWidth="24540" windowHeight="17540" activeTab="2" xr2:uid="{A8B7147D-77A5-1347-9728-F2522D06E352}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{A8B7147D-77A5-1347-9728-F2522D06E352}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="5" r:id="rId1"/>
     <sheet name="people" sheetId="2" r:id="rId2"/>
     <sheet name="projects" sheetId="3" r:id="rId3"/>
     <sheet name="funding" sheetId="4" r:id="rId4"/>
-    <sheet name="projects_x" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,47 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="337">
-  <si>
-    <t>Sequence space</t>
-  </si>
-  <si>
-    <t>![sequence space](img/seq_space.png)</t>
-  </si>
-  <si>
-    <t>An evolving protein must traverse sequence space</t>
-  </si>
-  <si>
-    <t>Epistasis (when mutations interact with one another) changes which pathways are accessible.</t>
-  </si>
-  <si>
-    <t>We found that...</t>
-  </si>
-  <si>
-    <t>Current projects</t>
-  </si>
-  <si>
-    <t>Can we use the signal from epistasis to dissect the biophysics of these maps?</t>
-  </si>
-  <si>
-    <t>Can we predict phenotypes given information from a small number of genotypes?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="301">
   <si>
     <t>Evolution of innate immune proteins</t>
   </si>
   <si>
-    <t>The innate immune system consists of multiple, interacting parts.</t>
-  </si>
-  <si>
-    <t>img/tlr4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + How did each of these parts evolve their functions in innate immunity?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + How does S100A9 activate TLR4?</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -255,78 +218,6 @@
     <t>Jaclyn Smith</t>
   </si>
   <si>
-    <t>We found that…</t>
-  </si>
-  <si>
-    <t>(... high-order epistasis shapes evolutionary trajectories.)[http://journals.plos.org/ploscompbiol/article?rev=2&amp;id=10.1371/journal.pcbi.1005541]</t>
-  </si>
-  <si>
-    <t>(..."high-order" epistasis (multi-way interactions between mutations) are ubiquitous in experimental sequence spaces.)[http://www.genetics.org/content/205/3/1079]</t>
-  </si>
-  <si>
-    <t>(... high-order epistasis is a natural consequence of the thermodynamic ensemble populated by proteins.)[http://www.pnas.org/content/114/45/11938.short]</t>
-  </si>
-  <si>
-    <t>(... useful epistatic coefficients cannot be resolved from sequence spaces using linear models.)[https://www.biorxiv.org/content/early/2018/07/27/378489]</t>
-  </si>
-  <si>
-    <t>(...S100A9 evolved multifunctionality through a pleiotropic substitution.)[https://elifesciences.org/articles/54100]</t>
-  </si>
-  <si>
-    <t>(... S100A9 activates TLR4 in a Zn(II)-independent fashion.)[https://www.biorxiv.org/content/10.1101/796219v1]</t>
-  </si>
-  <si>
-    <t>(... TLR4 evolved in the ancestor of bony vertebrates.  Zebrafish TLR4 responds to the same signals that activate human TLR4.)[https://www.biorxiv.org/content/10.1101/817528v1]</t>
-  </si>
-  <si>
-    <t>(... the human TLR4/MD-2 complex has--since the human-mouse ancestor--evolved new specificity for pro-inflammatory signals.)[https://onlinelibrary.wiley.com/doi/full/10.1002/pro.3644]</t>
-  </si>
-  <si>
-    <t>(... an early calgranulin evolved in the amniote ancestor interacts non-specifically with TLR4.)[https://www.frontiersin.org/articles/10.3389/fimmu.2018.00304/full]</t>
-  </si>
-  <si>
-    <t>What is the mechanism by which calgranulins activate TLR4?</t>
-  </si>
-  <si>
-    <t>How did the calprotectin heterodimer evolve from an ancestral homodimer?</t>
-  </si>
-  <si>
-    <t>Evolution of specificity</t>
-  </si>
-  <si>
-    <t>S100 proteins are small signaling proteins</t>
-  </si>
-  <si>
-    <t>They bind to metals and downstream peptide regions of protein targets</t>
-  </si>
-  <si>
-    <t>How did the metal and peptide binding specificity of these target proteins evolve?</t>
-  </si>
-  <si>
-    <t>img/s100</t>
-  </si>
-  <si>
-    <t>(...transition metal binding is a conserved feature, shared by most S100 proteins, but the residues in the binding site are highly labile.)[]</t>
-  </si>
-  <si>
-    <t>(...S100 proteins evolved in the ancestor of animals with spinal cords.)[]</t>
-  </si>
-  <si>
-    <t>(...although S100A5 and S100A6 bind to an extraordinary variety of target peptides, this set of targets has been conserved for 320 million years.)[]</t>
-  </si>
-  <si>
-    <t>(...ancestral proteins may not be generally less specific than modern proteins.)[https://www.biorxiv.org/content/10.1101/2020.05.27.120261v1]</t>
-  </si>
-  <si>
-    <t>(…we can use machine learning to determine binding "rules" for low-specificity proteins)[https://www.biorxiv.org/content/10.1101/2020.06.02.131086v1]</t>
-  </si>
-  <si>
-    <t>Define the set of biological targets for S100A5 and S100A6.</t>
-  </si>
-  <si>
-    <t>What are the chemical "rules" that these low-specificity proteins use to discriminate targets?</t>
-  </si>
-  <si>
     <t>Visiting Masters Student</t>
   </si>
   <si>
@@ -378,15 +269,6 @@
     <t>Experimental studies of biophysical basis of high-order epistasis</t>
   </si>
   <si>
-    <t>project</t>
-  </si>
-  <si>
-    <t>row1</t>
-  </si>
-  <si>
-    <t>row2</t>
-  </si>
-  <si>
     <t>anderson_circle_150x150.png</t>
   </si>
   <si>
@@ -1048,6 +930,15 @@
   </si>
   <si>
     <t>teaching.html</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2020.08.30.274340</t>
+  </si>
+  <si>
+    <t>Nixon CF, Lim SA, Sailer ZR, Zheludev IN, Gee CL, Kelch BA, Harms MJ, Marqusee S</t>
+  </si>
+  <si>
+    <t>Exploring the evolutionary history of kinetic stability in the alpha-lytic protease family</t>
   </si>
 </sst>
 </file>
@@ -1099,11 +990,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1424,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC076B7-4CEB-C143-9E7B-9F55AFCD75D9}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1443,737 +1332,757 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
       <c r="E1" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="F1" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="G1" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>318</v>
+        <v>279</v>
       </c>
       <c r="C2" t="s">
-        <v>319</v>
+        <v>280</v>
       </c>
       <c r="D2">
         <v>2003</v>
       </c>
       <c r="E2" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
-        <v>320</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>327</v>
+        <v>281</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
+        <v>276</v>
       </c>
       <c r="C3" t="s">
-        <v>316</v>
+        <v>277</v>
       </c>
       <c r="D3">
         <v>2005</v>
       </c>
       <c r="E3" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="F3" t="s">
-        <v>317</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>326</v>
+        <v>278</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>312</v>
+        <v>273</v>
       </c>
       <c r="C4" t="s">
-        <v>313</v>
+        <v>274</v>
       </c>
       <c r="D4">
         <v>2008</v>
       </c>
       <c r="E4" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="F4" t="s">
-        <v>314</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>325</v>
+        <v>275</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>309</v>
+        <v>270</v>
       </c>
       <c r="C5" t="s">
-        <v>310</v>
+        <v>271</v>
       </c>
       <c r="D5">
         <v>2009</v>
       </c>
       <c r="E5" t="s">
-        <v>293</v>
+        <v>254</v>
       </c>
       <c r="F5" t="s">
-        <v>311</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>324</v>
+        <v>272</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>239</v>
       </c>
       <c r="C6" t="s">
-        <v>307</v>
+        <v>268</v>
       </c>
       <c r="D6">
         <v>2010</v>
       </c>
       <c r="E6" t="s">
-        <v>264</v>
+        <v>225</v>
       </c>
       <c r="F6" t="s">
-        <v>308</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>323</v>
+        <v>269</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>305</v>
+        <v>266</v>
       </c>
       <c r="C7" t="s">
-        <v>304</v>
+        <v>265</v>
       </c>
       <c r="D7">
         <v>2010</v>
       </c>
       <c r="E7" t="s">
-        <v>275</v>
+        <v>236</v>
       </c>
       <c r="F7" t="s">
-        <v>306</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>322</v>
+        <v>267</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>301</v>
+        <v>262</v>
       </c>
       <c r="C8" t="s">
-        <v>302</v>
+        <v>263</v>
       </c>
       <c r="D8">
         <v>2011</v>
       </c>
       <c r="E8" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="F8" t="s">
-        <v>303</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>321</v>
+        <v>264</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>299</v>
+        <v>260</v>
       </c>
       <c r="C9" t="s">
-        <v>296</v>
+        <v>257</v>
       </c>
       <c r="D9">
         <v>2012</v>
       </c>
       <c r="E9" t="s">
-        <v>297</v>
+        <v>258</v>
       </c>
       <c r="F9" t="s">
-        <v>298</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>300</v>
+        <v>259</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s">
-        <v>291</v>
+        <v>252</v>
       </c>
       <c r="D10">
         <v>2013</v>
       </c>
       <c r="E10" t="s">
-        <v>293</v>
+        <v>254</v>
       </c>
       <c r="F10" t="s">
-        <v>294</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>295</v>
+        <v>255</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>278</v>
+        <v>239</v>
       </c>
       <c r="C11" t="s">
-        <v>287</v>
+        <v>248</v>
       </c>
       <c r="D11">
         <v>2013</v>
       </c>
       <c r="E11" t="s">
-        <v>288</v>
+        <v>249</v>
       </c>
       <c r="F11" t="s">
-        <v>289</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>290</v>
+        <v>250</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
-        <v>284</v>
+        <v>245</v>
       </c>
       <c r="C12" t="s">
-        <v>285</v>
+        <v>246</v>
       </c>
       <c r="D12">
         <v>2013</v>
       </c>
       <c r="E12" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="F12" t="s">
-        <v>283</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>282</v>
+        <v>244</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B13" t="s">
-        <v>278</v>
+        <v>239</v>
       </c>
       <c r="C13" t="s">
-        <v>277</v>
+        <v>238</v>
       </c>
       <c r="D13">
         <v>2014</v>
       </c>
       <c r="E13" t="s">
-        <v>279</v>
+        <v>240</v>
       </c>
       <c r="F13" t="s">
-        <v>280</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>281</v>
+        <v>241</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
-        <v>272</v>
+        <v>233</v>
       </c>
       <c r="C14" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="D14">
         <v>2014</v>
       </c>
       <c r="E14" t="s">
-        <v>275</v>
+        <v>236</v>
       </c>
       <c r="F14" t="s">
-        <v>274</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>286</v>
+        <v>235</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B15" t="s">
-        <v>262</v>
+        <v>223</v>
       </c>
       <c r="C15" t="s">
-        <v>263</v>
+        <v>224</v>
       </c>
       <c r="D15">
         <v>2016</v>
       </c>
       <c r="E15" t="s">
-        <v>264</v>
+        <v>225</v>
       </c>
       <c r="F15" t="s">
-        <v>265</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>266</v>
+        <v>226</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
-        <v>254</v>
+        <v>215</v>
       </c>
       <c r="C16" t="s">
-        <v>253</v>
+        <v>214</v>
       </c>
       <c r="D16">
         <v>2016</v>
       </c>
       <c r="E16" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="F16" t="s">
-        <v>255</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>256</v>
+        <v>216</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" t="s">
         <v>210</v>
       </c>
-      <c r="B17" t="s">
-        <v>249</v>
-      </c>
       <c r="C17" t="s">
-        <v>248</v>
+        <v>209</v>
       </c>
       <c r="D17">
         <v>2016</v>
       </c>
       <c r="E17" t="s">
-        <v>250</v>
+        <v>211</v>
       </c>
       <c r="F17" t="s">
-        <v>251</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>252</v>
+        <v>212</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>228</v>
       </c>
       <c r="C18" t="s">
-        <v>268</v>
+        <v>229</v>
       </c>
       <c r="D18">
         <v>2017</v>
       </c>
       <c r="E18" t="s">
-        <v>269</v>
+        <v>230</v>
       </c>
       <c r="F18" t="s">
-        <v>270</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>271</v>
+        <v>231</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B19" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="C19" t="s">
-        <v>244</v>
+        <v>205</v>
       </c>
       <c r="D19">
         <v>2017</v>
       </c>
       <c r="E19" t="s">
-        <v>245</v>
+        <v>206</v>
       </c>
       <c r="F19" t="s">
-        <v>246</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>247</v>
+        <v>207</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B20" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="C20" t="s">
-        <v>241</v>
+        <v>202</v>
       </c>
       <c r="D20">
         <v>2017</v>
       </c>
       <c r="E20" t="s">
-        <v>242</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>243</v>
+        <v>203</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="C21" t="s">
-        <v>235</v>
+        <v>196</v>
       </c>
       <c r="D21">
         <v>2017</v>
       </c>
       <c r="E21" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="F21" t="s">
-        <v>238</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>239</v>
+        <v>199</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B22" t="s">
-        <v>234</v>
+        <v>195</v>
       </c>
       <c r="C22" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
       <c r="D22">
         <v>2017</v>
       </c>
       <c r="E22" t="s">
-        <v>232</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>233</v>
+        <v>193</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B23" t="s">
-        <v>260</v>
+        <v>221</v>
       </c>
       <c r="C23" t="s">
-        <v>257</v>
+        <v>218</v>
       </c>
       <c r="D23">
         <v>2018</v>
       </c>
       <c r="E23" t="s">
-        <v>258</v>
+        <v>219</v>
       </c>
       <c r="F23" t="s">
-        <v>259</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>261</v>
+        <v>220</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
-        <v>328</v>
+        <v>289</v>
       </c>
       <c r="C24" t="s">
-        <v>228</v>
+        <v>189</v>
       </c>
       <c r="D24">
         <v>2018</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>229</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>230</v>
+        <v>190</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B25" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
       <c r="C25" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="D25">
         <v>2018</v>
       </c>
       <c r="E25" t="s">
-        <v>226</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>227</v>
+        <v>187</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B26" t="s">
-        <v>221</v>
+        <v>182</v>
       </c>
       <c r="C26" t="s">
-        <v>220</v>
+        <v>181</v>
       </c>
       <c r="D26">
         <v>2018</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>222</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>223</v>
+        <v>183</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B27" t="s">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="C27" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="D27">
         <v>2019</v>
       </c>
       <c r="E27" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="F27" t="s">
-        <v>218</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>219</v>
+        <v>179</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="B28" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="C28" t="s">
-        <v>208</v>
+        <v>169</v>
       </c>
       <c r="D28">
         <v>2020</v>
       </c>
       <c r="E28" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="F28" t="s">
-        <v>212</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>213</v>
+        <v>173</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>331</v>
+        <v>292</v>
       </c>
       <c r="B29" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="C29" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="D29">
         <v>2020</v>
       </c>
       <c r="E29" t="s">
-        <v>242</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="B30" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="D30">
         <v>2019</v>
       </c>
       <c r="E30" t="s">
-        <v>194</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>204</v>
+        <v>155</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>329</v>
+        <v>290</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="D31">
         <v>2019</v>
       </c>
       <c r="E31" t="s">
-        <v>194</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>197</v>
+        <v>155</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="C32" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="D32">
         <v>2020</v>
       </c>
       <c r="E32" t="s">
-        <v>194</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>202</v>
+        <v>155</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>330</v>
+        <v>291</v>
       </c>
       <c r="B33" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="C33" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="D33">
         <v>2020</v>
       </c>
       <c r="E33" t="s">
-        <v>194</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>196</v>
+        <v>155</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>290</v>
+      </c>
+      <c r="B34" t="s">
+        <v>299</v>
+      </c>
+      <c r="C34" t="s">
+        <v>300</v>
+      </c>
+      <c r="D34">
+        <v>2020</v>
+      </c>
+      <c r="E34" t="s">
+        <v>155</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2209,6 +2118,7 @@
     <hyperlink ref="G4" r:id="rId29" xr:uid="{4E06EB98-A16A-5440-B604-68B41286E37E}"/>
     <hyperlink ref="G3" r:id="rId30" xr:uid="{79FA9F8C-B50B-9A45-AB12-7B8902450FEE}"/>
     <hyperlink ref="G2" r:id="rId31" xr:uid="{6E3F39B4-F9C2-2E49-A744-DE4788D59A56}"/>
+    <hyperlink ref="G34" r:id="rId32" xr:uid="{5524E091-EA10-5B42-AC63-A8D32A2E716B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2237,537 +2147,537 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
       <c r="J1" t="s">
-        <v>153</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>78</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>79</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>34</v>
+        <v>81</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>143</v>
+        <v>82</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>154</v>
+        <v>84</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="E8" t="s">
-        <v>124</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>146</v>
+        <v>85</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>149</v>
+        <v>88</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="H14" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>332</v>
+        <v>293</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>116</v>
+        <v>77</v>
       </c>
       <c r="F15" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
-      </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>134</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="H19" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="F21" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>106</v>
+        <v>69</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E22" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>139</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
         <v>42</v>
       </c>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>54</v>
-      </c>
       <c r="E25" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>141</v>
+        <v>102</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2797,7 +2707,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2809,68 +2719,68 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
-        <v>333</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>334</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>335</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
-        <v>336</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -2883,7 +2793,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2896,33 +2806,33 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>176</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>183</v>
+        <v>128</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2930,16 +2840,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>184</v>
+        <v>140</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2947,16 +2857,16 @@
     </row>
     <row r="4" spans="1:5" ht="17">
       <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>189</v>
+        <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>185</v>
+        <v>139</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2964,16 +2874,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>186</v>
+        <v>136</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2981,16 +2891,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>187</v>
+        <v>141</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2998,16 +2908,16 @@
     </row>
     <row r="7" spans="1:5" ht="17">
       <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>172</v>
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>188</v>
+        <v>138</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3015,16 +2925,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
+        <v>134</v>
       </c>
       <c r="C8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>181</v>
+        <v>128</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3032,16 +2942,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>182</v>
+        <v>128</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -3060,293 +2970,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D72B0B-0937-4247-A733-A86715609C32}">
-  <dimension ref="A1:C28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="143.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>3</v>
-      </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated shavlik pic, tried to fix ipad bg
</commit_message>
<xml_diff>
--- a/source/pages.xlsx
+++ b/source/pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/admin/website/github/website/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E91007-B740-A14B-8FF4-70236A08F548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4544F66F-CC05-0B4C-9F45-10EB8F12A621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{A8B7147D-77A5-1347-9728-F2522D06E352}"/>
+    <workbookView xWindow="36600" yWindow="-1500" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{A8B7147D-77A5-1347-9728-F2522D06E352}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="5" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t>Jeremy Anderson</t>
   </si>
   <si>
-    <t>Data scientist</t>
-  </si>
-  <si>
     <t>Nick Frantz</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>Zach Sailer</t>
   </si>
   <si>
-    <t>Software developer, Jupyter project</t>
-  </si>
-  <si>
     <t>Caitlyn Wong</t>
   </si>
   <si>
@@ -939,6 +933,12 @@
   </si>
   <si>
     <t>Exploring the evolutionary history of kinetic stability in the alpha-lytic protease family</t>
+  </si>
+  <si>
+    <t>Software developer, Apple</t>
+  </si>
+  <si>
+    <t>Data scientist, Travelers Insurance</t>
   </si>
 </sst>
 </file>
@@ -1335,536 +1335,536 @@
         <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" t="s">
         <v>154</v>
       </c>
-      <c r="F1" t="s">
-        <v>156</v>
-      </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D2">
         <v>2003</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D3">
         <v>2005</v>
       </c>
       <c r="E3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D4">
         <v>2008</v>
       </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D5">
         <v>2009</v>
       </c>
       <c r="E5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D6">
         <v>2010</v>
       </c>
       <c r="E6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D7">
         <v>2010</v>
       </c>
       <c r="E7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D8">
         <v>2011</v>
       </c>
       <c r="E8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D9">
         <v>2012</v>
       </c>
       <c r="E9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F9" t="s">
+        <v>257</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D10">
         <v>2013</v>
       </c>
       <c r="E10" t="s">
+        <v>252</v>
+      </c>
+      <c r="F10" t="s">
+        <v>253</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="F10" t="s">
-        <v>255</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D11">
         <v>2013</v>
       </c>
       <c r="E11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" t="s">
+        <v>248</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="F11" t="s">
-        <v>250</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D12">
         <v>2013</v>
       </c>
       <c r="E12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D13">
         <v>2014</v>
       </c>
       <c r="E13" t="s">
+        <v>238</v>
+      </c>
+      <c r="F13" t="s">
+        <v>239</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F13" t="s">
-        <v>241</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D14">
         <v>2014</v>
       </c>
       <c r="E14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D15">
         <v>2016</v>
       </c>
       <c r="E15" t="s">
+        <v>223</v>
+      </c>
+      <c r="F15" t="s">
+        <v>224</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="F15" t="s">
-        <v>226</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D16">
         <v>2016</v>
       </c>
       <c r="E16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D17">
         <v>2016</v>
       </c>
       <c r="E17" t="s">
+        <v>209</v>
+      </c>
+      <c r="F17" t="s">
+        <v>210</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="F17" t="s">
-        <v>212</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D18">
         <v>2017</v>
       </c>
       <c r="E18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F18" t="s">
+        <v>229</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="F18" t="s">
-        <v>231</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D19">
         <v>2017</v>
       </c>
       <c r="E19" t="s">
+        <v>204</v>
+      </c>
+      <c r="F19" t="s">
+        <v>205</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="F19" t="s">
-        <v>207</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D20">
         <v>2017</v>
       </c>
       <c r="E20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D21">
         <v>2017</v>
       </c>
       <c r="E21" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" t="s">
+        <v>197</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="F21" t="s">
-        <v>199</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D22">
         <v>2017</v>
       </c>
       <c r="E22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D23">
         <v>2018</v>
       </c>
       <c r="E23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F23" t="s">
+        <v>218</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B24" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D24">
         <v>2018</v>
@@ -1873,41 +1873,41 @@
         <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D25">
         <v>2018</v>
       </c>
       <c r="E25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D26">
         <v>2018</v>
@@ -1916,173 +1916,173 @@
         <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D27">
         <v>2019</v>
       </c>
       <c r="E27" t="s">
+        <v>175</v>
+      </c>
+      <c r="F27" t="s">
         <v>177</v>
       </c>
-      <c r="F27" t="s">
-        <v>179</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D28">
         <v>2020</v>
       </c>
       <c r="E28" t="s">
+        <v>170</v>
+      </c>
+      <c r="F28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="F28" t="s">
-        <v>173</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D29">
         <v>2020</v>
       </c>
       <c r="E29" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C30" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D30">
         <v>2019</v>
       </c>
       <c r="E30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D31">
         <v>2019</v>
       </c>
       <c r="E31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B32" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" t="s">
         <v>160</v>
-      </c>
-      <c r="C32" t="s">
-        <v>162</v>
       </c>
       <c r="D32">
         <v>2020</v>
       </c>
       <c r="E32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D33">
         <v>2020</v>
       </c>
       <c r="E33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B34" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C34" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D34">
         <v>2020</v>
       </c>
       <c r="E34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -2128,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A604AB1-DDFC-4B40-85A4-D0BC5335EE4C}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2174,7 +2174,7 @@
         <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2191,7 +2191,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -2214,15 +2214,15 @@
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -2240,7 +2240,7 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>17</v>
@@ -2260,7 +2260,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>22</v>
@@ -2280,13 +2280,13 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2294,25 +2294,25 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="E7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2326,13 +2326,13 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2340,16 +2340,16 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2360,13 +2360,13 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2380,19 +2380,19 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2409,7 +2409,7 @@
         <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2426,7 +2426,7 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2434,19 +2434,19 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2457,19 +2457,19 @@
         <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>300</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2477,16 +2477,16 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2494,13 +2494,13 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2508,16 +2508,16 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
         <v>44</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>45</v>
       </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2525,25 +2525,25 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>299</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" t="s">
         <v>65</v>
-      </c>
-      <c r="G19" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2551,19 +2551,19 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2571,22 +2571,22 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
         <v>50</v>
       </c>
-      <c r="C21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" t="s">
-        <v>52</v>
-      </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2594,7 +2594,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -2603,7 +2603,7 @@
         <v>35</v>
       </c>
       <c r="E22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2611,16 +2611,16 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2628,7 +2628,7 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
@@ -2637,13 +2637,13 @@
         <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2651,16 +2651,16 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2668,16 +2668,16 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2706,7 +2706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DD845D-47E5-1E42-A12B-67B3BEB52BF9}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2725,62 +2725,62 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -2815,10 +2815,10 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2826,13 +2826,13 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2843,13 +2843,13 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2860,13 +2860,13 @@
         <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2877,13 +2877,13 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2894,13 +2894,13 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2911,13 +2911,13 @@
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2928,13 +2928,13 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2945,13 +2945,13 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E9">
         <v>1</v>

</xml_diff>

<commit_message>
fixed bad linkedin link
</commit_message>
<xml_diff>
--- a/source/pages.xlsx
+++ b/source/pages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/admin/website/github/website/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F935767-7BA7-564C-A015-274A7A489810}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D37B8F3-AC0B-CC44-8717-B1669294AD75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A8B7147D-77A5-1347-9728-F2522D06E352}"/>
   </bookViews>
@@ -1355,7 +1355,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2193,8 +2193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A604AB1-DDFC-4B40-85A4-D0BC5335EE4C}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2310,9 +2310,6 @@
       <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>313</v>
-      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2355,6 +2352,9 @@
       </c>
       <c r="H6" s="1" t="s">
         <v>312</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -2807,7 +2807,7 @@
     <hyperlink ref="J8" r:id="rId15" xr:uid="{7AD87150-852A-EC48-8A33-35899592670A}"/>
     <hyperlink ref="H12" r:id="rId16" display="mailto:Jyin5@uoregon.edu" xr:uid="{BD89C2C8-01DA-0945-8C45-44FC2597E1A0}"/>
     <hyperlink ref="H6" r:id="rId17" display="mailto:konao@uoregon.edu" xr:uid="{99A77FB4-F7EA-7A4E-A1D6-82B0846E355F}"/>
-    <hyperlink ref="J4" r:id="rId18" display="http://www.linkedin.com/in/kona-orlandi" xr:uid="{72314501-811D-D043-997F-E392845F576D}"/>
+    <hyperlink ref="J6" r:id="rId18" display="http://www.linkedin.com/in/kona-orlandi" xr:uid="{72314501-811D-D043-997F-E392845F576D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated pubs, mastadon links
</commit_message>
<xml_diff>
--- a/source/pages.xlsx
+++ b/source/pages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/admin/website/website/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32775E7-FF8F-B744-A3C8-868171FD9277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C70476-6FFE-4341-9E7C-705199B7A39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{A8B7147D-77A5-1347-9728-F2522D06E352}"/>
+    <workbookView xWindow="-34080" yWindow="2540" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{A8B7147D-77A5-1347-9728-F2522D06E352}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="363">
   <si>
     <t>Evolution of innate immune proteins</t>
   </si>
@@ -1052,9 +1052,6 @@
     <t>Jose Sanchez-Borbon</t>
   </si>
   <si>
-    <t>Evolution of CD14 in fishes</t>
-  </si>
-  <si>
     <t>Morrision AJ, Harms MJ</t>
   </si>
   <si>
@@ -1089,6 +1086,45 @@
   </si>
   <si>
     <t>Harman JL, Reardon PN, Costello SM, Warren GD, Phillips SR, Connor PJ, Marqusee S, Harms MJ</t>
+  </si>
+  <si>
+    <t>How did the CD14 LPS binding site evolve?</t>
+  </si>
+  <si>
+    <t>in press</t>
+  </si>
+  <si>
+    <t>Topiary: pruning the manual labor from ancestral sequence reconstruction</t>
+  </si>
+  <si>
+    <t>Orlandi KN, Phillips SR, Sailer ZR, Harman JL, Harms MJ</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/pro.4551</t>
+  </si>
+  <si>
+    <t>Morin MA, Morrison AJ, Harms MJ, Dutton RJ</t>
+  </si>
+  <si>
+    <t>Higher-order interactions shape microbial interactions as microbial community complexity increases</t>
+  </si>
+  <si>
+    <t>Scientific Reports</t>
+  </si>
+  <si>
+    <t>12: 22640</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41598-022-25303-1</t>
+  </si>
+  <si>
+    <t>Biophysical Journal</t>
+  </si>
+  <si>
+    <t>mastadon</t>
+  </si>
+  <si>
+    <t>https://ecoevo.social/@EvolBiochemist</t>
   </si>
 </sst>
 </file>
@@ -1464,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC076B7-4CEB-C143-9E7B-9F55AFCD75D9}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2348,10 +2384,10 @@
         <v>161</v>
       </c>
       <c r="B39" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C39" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D39">
         <v>2022</v>
@@ -2360,50 +2396,93 @@
         <v>188</v>
       </c>
       <c r="F39" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>304</v>
+        <v>161</v>
       </c>
       <c r="B40" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="C40" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="D40">
         <v>2022</v>
       </c>
       <c r="E40" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>304</v>
+        <v>161</v>
       </c>
       <c r="B41" t="s">
-        <v>339</v>
+        <v>355</v>
       </c>
       <c r="C41" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="D41">
         <v>2022</v>
       </c>
       <c r="E41" t="s">
+        <v>357</v>
+      </c>
+      <c r="F41" t="s">
+        <v>358</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>351</v>
+      </c>
+      <c r="B42" t="s">
+        <v>339</v>
+      </c>
+      <c r="C42" t="s">
+        <v>340</v>
+      </c>
+      <c r="D42">
+        <v>2022</v>
+      </c>
+      <c r="E42" t="s">
+        <v>360</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>304</v>
+      </c>
+      <c r="B43" t="s">
+        <v>338</v>
+      </c>
+      <c r="C43" t="s">
+        <v>343</v>
+      </c>
+      <c r="D43">
+        <v>2022</v>
+      </c>
+      <c r="E43" t="s">
         <v>149</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>343</v>
+      <c r="G43" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2443,9 +2522,11 @@
     <hyperlink ref="G31" r:id="rId33" xr:uid="{F10C0FAD-F8FD-BD43-AC40-575582642BD8}"/>
     <hyperlink ref="G37" r:id="rId34" xr:uid="{05A31E51-E542-2E4D-BF23-E76318417D1C}"/>
     <hyperlink ref="G38" r:id="rId35" xr:uid="{A83E1A5F-F28D-9D48-B99B-2A40390E67E4}"/>
-    <hyperlink ref="G40" r:id="rId36" xr:uid="{D23694B0-2E8C-5C4D-AA39-FFA20FA00800}"/>
-    <hyperlink ref="G41" r:id="rId37" xr:uid="{1654A9D4-65E8-9F4F-8DE2-4A51E8C5F1FA}"/>
-    <hyperlink ref="G39" r:id="rId38" xr:uid="{322824A7-B8BE-CE4A-9140-04CF199293F0}"/>
+    <hyperlink ref="G39" r:id="rId36" xr:uid="{322824A7-B8BE-CE4A-9140-04CF199293F0}"/>
+    <hyperlink ref="G41" r:id="rId37" xr:uid="{75414802-46F0-FB4F-AB5B-746E343B5310}"/>
+    <hyperlink ref="G40" r:id="rId38" xr:uid="{D121D190-6997-DE49-B711-B0A0F985B6AC}"/>
+    <hyperlink ref="G42" r:id="rId39" xr:uid="{79020FD8-1031-EE4E-AD55-E6B083D09D45}"/>
+    <hyperlink ref="G43" r:id="rId40" xr:uid="{22036C22-E126-FF4D-B5AB-64C14DF4FB9F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2453,10 +2534,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A604AB1-DDFC-4B40-85A4-D0BC5335EE4C}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2467,12 +2548,13 @@
     <col min="4" max="4" width="90.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -2492,19 +2574,22 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>361</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -2524,13 +2609,16 @@
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2548,12 +2636,13 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2569,14 +2658,14 @@
       <c r="E4" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -2592,14 +2681,14 @@
       <c r="E5" t="s">
         <v>300</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -2615,11 +2704,11 @@
       <c r="E6" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2638,14 +2727,15 @@
       <c r="F7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="G7" s="1"/>
+      <c r="I7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -2661,11 +2751,11 @@
       <c r="E8" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2676,16 +2766,16 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
       <c r="E9" t="s">
+        <v>344</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -2701,11 +2791,11 @@
       <c r="E10" t="s">
         <v>296</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2721,11 +2811,11 @@
       <c r="E11" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2742,7 +2832,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2759,7 +2849,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -2778,14 +2868,15 @@
       <c r="F14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2802,7 +2893,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2819,7 +2910,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2835,11 +2926,11 @@
       <c r="E17" t="s">
         <v>84</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2858,11 +2949,11 @@
       <c r="F18" t="s">
         <v>60</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -2879,7 +2970,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2893,7 +2984,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2910,7 +3001,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2929,14 +3020,15 @@
       <c r="F22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="2"/>
+      <c r="H22" t="s">
         <v>63</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -2952,11 +3044,11 @@
       <c r="E23" t="s">
         <v>91</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2975,11 +3067,11 @@
       <c r="F24" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2996,7 +3088,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -3013,7 +3105,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -3032,11 +3124,12 @@
       <c r="F27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="1"/>
+      <c r="H27" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -3053,7 +3146,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3076,24 +3169,25 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{1DE0CD26-AAF6-C14D-AC57-1E20477BBEF9}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{4B69F9D1-9BDC-3B49-95D5-B892E0F38E93}"/>
-    <hyperlink ref="G11" r:id="rId3" xr:uid="{F297B546-961A-904C-8B57-270571840D4C}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{82F2EFE6-4E28-F34E-B218-DAA2AC17ECFE}"/>
-    <hyperlink ref="G24" r:id="rId5" xr:uid="{B5F9801A-D1FF-F945-B5EA-A95297A9AC9E}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{4B69F9D1-9BDC-3B49-95D5-B892E0F38E93}"/>
+    <hyperlink ref="H11" r:id="rId3" xr:uid="{F297B546-961A-904C-8B57-270571840D4C}"/>
+    <hyperlink ref="I4" r:id="rId4" xr:uid="{82F2EFE6-4E28-F34E-B218-DAA2AC17ECFE}"/>
+    <hyperlink ref="H24" r:id="rId5" xr:uid="{B5F9801A-D1FF-F945-B5EA-A95297A9AC9E}"/>
     <hyperlink ref="F27" r:id="rId6" xr:uid="{7C843EC2-4C8D-4641-BB36-2B0270ADEE55}"/>
-    <hyperlink ref="H3" r:id="rId7" xr:uid="{B1C6FFD0-CEC7-F545-85D8-C469FD54EC40}"/>
-    <hyperlink ref="H6" r:id="rId8" xr:uid="{0B982E49-986A-0941-8C32-ADEAA21D9033}"/>
-    <hyperlink ref="H7" r:id="rId9" xr:uid="{82A7CA40-D4B3-CD48-B0DD-40DB2C17FB15}"/>
+    <hyperlink ref="I3" r:id="rId7" xr:uid="{B1C6FFD0-CEC7-F545-85D8-C469FD54EC40}"/>
+    <hyperlink ref="I6" r:id="rId8" xr:uid="{0B982E49-986A-0941-8C32-ADEAA21D9033}"/>
+    <hyperlink ref="I7" r:id="rId9" xr:uid="{82A7CA40-D4B3-CD48-B0DD-40DB2C17FB15}"/>
     <hyperlink ref="F7" r:id="rId10" xr:uid="{DBABC5AF-727A-5F45-976D-9D37304F647C}"/>
-    <hyperlink ref="H8" r:id="rId11" xr:uid="{D81BC1A6-DB5E-2442-8092-0DCC05080E7B}"/>
+    <hyperlink ref="I8" r:id="rId11" xr:uid="{D81BC1A6-DB5E-2442-8092-0DCC05080E7B}"/>
     <hyperlink ref="F14" r:id="rId12" xr:uid="{671646BC-4048-784B-A41A-EE3B6A5872DF}"/>
-    <hyperlink ref="G14" r:id="rId13" xr:uid="{520C3AB8-D98F-5A41-A791-18E65C05A26D}"/>
-    <hyperlink ref="H14" r:id="rId14" xr:uid="{AC194642-8CCA-D045-8B43-2E593C852C84}"/>
-    <hyperlink ref="J7" r:id="rId15" xr:uid="{7AD87150-852A-EC48-8A33-35899592670A}"/>
-    <hyperlink ref="H10" r:id="rId16" display="mailto:Jyin5@uoregon.edu" xr:uid="{BD89C2C8-01DA-0945-8C45-44FC2597E1A0}"/>
-    <hyperlink ref="H5" r:id="rId17" display="mailto:konao@uoregon.edu" xr:uid="{99A77FB4-F7EA-7A4E-A1D6-82B0846E355F}"/>
-    <hyperlink ref="J5" r:id="rId18" xr:uid="{72314501-811D-D043-997F-E392845F576D}"/>
-    <hyperlink ref="H9" r:id="rId19" xr:uid="{3B7DC98F-564E-8040-ABB3-24351F91CBD2}"/>
+    <hyperlink ref="H14" r:id="rId13" xr:uid="{520C3AB8-D98F-5A41-A791-18E65C05A26D}"/>
+    <hyperlink ref="I14" r:id="rId14" xr:uid="{AC194642-8CCA-D045-8B43-2E593C852C84}"/>
+    <hyperlink ref="K7" r:id="rId15" xr:uid="{7AD87150-852A-EC48-8A33-35899592670A}"/>
+    <hyperlink ref="I10" r:id="rId16" display="mailto:Jyin5@uoregon.edu" xr:uid="{BD89C2C8-01DA-0945-8C45-44FC2597E1A0}"/>
+    <hyperlink ref="I5" r:id="rId17" display="mailto:konao@uoregon.edu" xr:uid="{99A77FB4-F7EA-7A4E-A1D6-82B0846E355F}"/>
+    <hyperlink ref="K5" r:id="rId18" xr:uid="{72314501-811D-D043-997F-E392845F576D}"/>
+    <hyperlink ref="I9" r:id="rId19" xr:uid="{3B7DC98F-564E-8040-ABB3-24351F91CBD2}"/>
+    <hyperlink ref="G2" r:id="rId20" xr:uid="{944B277E-1502-DF4C-99EE-2856B2C13CD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>